<commit_message>
Update LMS6 Interface BOM Rev C.xlsx
</commit_message>
<xml_diff>
--- a/Fabrication/LMS6 Interface BOM Rev C.xlsx
+++ b/Fabrication/LMS6 Interface BOM Rev C.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reid\Documents\KiCad Projects\Programmer Board\LMS-6_Interface_Board\Fabrication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF72E872-FB55-42E5-9080-836A7F2C9CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181DB2AE-7420-4AAB-A829-E4889F3CBA60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69C77648-9DF9-4609-9F16-FA709D4A2690}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
   <si>
     <t>Qty</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>Isolated Module DC DC Converter 1 Output 9V    222mA 4.5V - 18V Input</t>
+  </si>
+  <si>
+    <t>NPC02SXON-RC</t>
+  </si>
+  <si>
+    <t>2 (1 x 2) Position Shunt Connector  Open Top, Grip 0.100" (2.54mm) Gold</t>
   </si>
 </sst>
 </file>
@@ -354,13 +360,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C8952A2-E0F3-4B07-89C6-E352D8A40B74}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,7 +900,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -1128,6 +1138,24 @@
       </c>
       <c r="F22" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>